<commit_message>
Updated IR range data
</commit_message>
<xml_diff>
--- a/Testing/IR Sensor MNML Board Data.xlsx
+++ b/Testing/IR Sensor MNML Board Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6470"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="6310" windowHeight="6250"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Real distance</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t>Result</t>
+  </si>
+  <si>
+    <t>1/Result</t>
   </si>
 </sst>
 </file>
@@ -437,10 +440,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$94</c:f>
+              <c:f>Sheet1!$B$2:$B$91</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="93"/>
+                <c:ptCount val="90"/>
                 <c:pt idx="0">
                   <c:v>429</c:v>
                 </c:pt>
@@ -703,21 +706,12 @@
                   <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>88</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>85</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>105</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="92">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -733,11 +727,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="338835784"/>
-        <c:axId val="339694080"/>
+        <c:axId val="254970392"/>
+        <c:axId val="254973136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="338835784"/>
+        <c:axId val="254970392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -839,12 +833,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="339694080"/>
+        <c:crossAx val="254973136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="339694080"/>
+        <c:axId val="254973136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -946,7 +940,913 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="338835784"/>
+        <c:crossAx val="254970392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Invert</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.31274039718933622"/>
+                  <c:y val="0.11961630524732829"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="0.000000E+00" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$14:$A$94</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="81"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>140</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$14:$C$94</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="81"/>
+                <c:pt idx="0">
+                  <c:v>1.7513134851138354E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7482517482517483E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7094017094017094E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8181818181818182E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8050541516245488E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.8518518518518519E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.1052631578947368E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.1141649048625794E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.1141649048625794E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.3201856148491878E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.3148148148148147E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.352941176470588E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.8169014084507044E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.8011204481792717E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.7855153203342618E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.0674846625766872E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.1250000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.1446540880503146E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.663003663003663E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.4965034965034965E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.6231884057971015E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.968253968253968E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.8910505836575876E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.4247787610619468E-3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.4052863436123352E-3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.3859649122807015E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.7393364928909956E-3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.6948356807511738E-3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.6511627906976744E-3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5.076142131979695E-3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.0505050505050509E-3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.0505050505050509E-3</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5.4945054945054949E-3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5.4644808743169399E-3</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5.4644808743169399E-3</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5.681818181818182E-3</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.7142857142857143E-3</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>5.7142857142857143E-3</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>6.2893081761006293E-3</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>6.1349693251533744E-3</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>5.681818181818182E-3</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>6.41025641025641E-3</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>6.2111801242236021E-3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>6.0975609756097563E-3</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>6.9444444444444441E-3</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>6.9444444444444441E-3</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>6.8027210884353739E-3</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>8.0000000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>7.4074074074074077E-3</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>7.462686567164179E-3</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>7.4074074074074077E-3</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>7.3529411764705881E-3</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>7.6335877862595417E-3</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>8.130081300813009E-3</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>7.874015748031496E-3</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>7.8125E-3</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>8.130081300813009E-3</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>7.7519379844961239E-3</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>8.6956521739130436E-3</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>8.3333333333333332E-3</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>8.3333333333333332E-3</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>8.2644628099173556E-3</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>8.5470085470085479E-3</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>8.0645161290322578E-3</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>8.9285714285714281E-3</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.0752688172043012E-2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>9.0909090909090905E-3</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>8.9285714285714281E-3</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>8.5470085470085479E-3</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>9.0909090909090905E-3</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>9.6153846153846159E-3</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>9.7087378640776691E-3</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>9.3457943925233638E-3</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>9.5238095238095247E-3</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1.1764705882352941E-2</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1.1363636363636364E-2</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1.1764705882352941E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="312700104"/>
+        <c:axId val="312697360"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="312700104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="312697360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="312697360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="312700104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1067,6 +1967,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1583,20 +2523,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>224465</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>44303</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>354854</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>177427</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>73837</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>5613</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>140075</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>149411</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1610,6 +3066,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>277345</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>5789</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>196102</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>18676</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1883,12 +3369,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="43" workbookViewId="0">
-      <selection activeCell="AH27" sqref="AH27"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="11.7265625" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1896,8 +3383,11 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -1910,6 +3400,10 @@
       <c r="B2">
         <v>429</v>
       </c>
+      <c r="C2">
+        <f>1/B2</f>
+        <v>2.331002331002331E-3</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
@@ -1918,6 +3412,10 @@
       <c r="B3">
         <v>420</v>
       </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C66" si="0">1/B3</f>
+        <v>2.3809523809523812E-3</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
@@ -1926,6 +3424,10 @@
       <c r="B4">
         <v>400</v>
       </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-3</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
@@ -1934,6 +3436,10 @@
       <c r="B5">
         <v>417</v>
       </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>2.3980815347721821E-3</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
@@ -1942,6 +3448,10 @@
       <c r="B6">
         <v>418</v>
       </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>2.3923444976076554E-3</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
@@ -1950,6 +3460,10 @@
       <c r="B7">
         <v>421</v>
       </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>2.3752969121140144E-3</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
@@ -1958,6 +3472,10 @@
       <c r="B8">
         <v>435</v>
       </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>2.2988505747126436E-3</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
@@ -1966,6 +3484,10 @@
       <c r="B9">
         <v>439</v>
       </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>2.2779043280182231E-3</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
@@ -1974,6 +3496,10 @@
       <c r="B10">
         <v>436</v>
       </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>2.2935779816513763E-3</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
@@ -1982,6 +3508,10 @@
       <c r="B11">
         <v>534</v>
       </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>1.8726591760299626E-3</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
@@ -1990,6 +3520,10 @@
       <c r="B12">
         <v>526</v>
       </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>1.9011406844106464E-3</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
@@ -1998,6 +3532,10 @@
       <c r="B13">
         <v>522</v>
       </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>1.9157088122605363E-3</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
@@ -2006,6 +3544,10 @@
       <c r="B14">
         <v>571</v>
       </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>1.7513134851138354E-3</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
@@ -2014,6 +3556,10 @@
       <c r="B15">
         <v>572</v>
       </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>1.7482517482517483E-3</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
@@ -2022,629 +3568,945 @@
       <c r="B16">
         <v>585</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>1.7094017094017094E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>20</v>
       </c>
       <c r="B17">
         <v>550</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>1.8181818181818182E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>20</v>
       </c>
       <c r="B18">
         <v>554</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>1.8050541516245488E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>20</v>
       </c>
       <c r="B19">
         <v>540</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>1.8518518518518519E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>25</v>
       </c>
       <c r="B20">
         <v>475</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>2.1052631578947368E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>25</v>
       </c>
       <c r="B21">
         <v>473</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>2.1141649048625794E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>25</v>
       </c>
       <c r="B22">
         <v>473</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>2.1141649048625794E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>30</v>
       </c>
       <c r="B23">
         <v>431</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>2.3201856148491878E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>30</v>
       </c>
       <c r="B24">
         <v>432</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>2.3148148148148147E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>30</v>
       </c>
       <c r="B25">
         <v>425</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>2.352941176470588E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>35</v>
       </c>
       <c r="B26">
         <v>355</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>2.8169014084507044E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>35</v>
       </c>
       <c r="B27">
         <v>357</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>2.8011204481792717E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>35</v>
       </c>
       <c r="B28">
         <v>359</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>2.7855153203342618E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>40</v>
       </c>
       <c r="B29">
         <v>326</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>3.0674846625766872E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>40</v>
       </c>
       <c r="B30">
         <v>320</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>3.1250000000000002E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>40</v>
       </c>
       <c r="B31">
         <v>318</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>3.1446540880503146E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>45</v>
       </c>
       <c r="B32">
         <v>273</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>3.663003663003663E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>45</v>
       </c>
       <c r="B33">
         <v>286</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>3.4965034965034965E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>45</v>
       </c>
       <c r="B34">
         <v>276</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>3.6231884057971015E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>50</v>
       </c>
       <c r="B35">
         <v>252</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>3.968253968253968E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>50</v>
       </c>
       <c r="B36">
         <v>250</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>50</v>
       </c>
       <c r="B37">
         <v>257</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>3.8910505836575876E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>55</v>
       </c>
       <c r="B38">
         <v>226</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>4.4247787610619468E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>55</v>
       </c>
       <c r="B39">
         <v>227</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>4.4052863436123352E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>55</v>
       </c>
       <c r="B40">
         <v>228</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>4.3859649122807015E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>60</v>
       </c>
       <c r="B41">
         <v>211</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>4.7393364928909956E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>60</v>
       </c>
       <c r="B42">
         <v>213</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>4.6948356807511738E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>60</v>
       </c>
       <c r="B43">
         <v>215</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>4.6511627906976744E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>65</v>
       </c>
       <c r="B44">
         <v>197</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>5.076142131979695E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>65</v>
       </c>
       <c r="B45">
         <v>198</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>5.0505050505050509E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>65</v>
       </c>
       <c r="B46">
         <v>198</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>5.0505050505050509E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>70</v>
       </c>
       <c r="B47">
         <v>182</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>5.4945054945054949E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>70</v>
       </c>
       <c r="B48">
         <v>183</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>5.4644808743169399E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>70</v>
       </c>
       <c r="B49">
         <v>183</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>5.4644808743169399E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>75</v>
       </c>
       <c r="B50">
         <v>176</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>5.681818181818182E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>75</v>
       </c>
       <c r="B51">
         <v>175</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>5.7142857142857143E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>75</v>
       </c>
       <c r="B52">
         <v>175</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>5.7142857142857143E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>80</v>
       </c>
       <c r="B53">
         <v>159</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>6.2893081761006293E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>80</v>
       </c>
       <c r="B54">
         <v>163</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>6.1349693251533744E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>80</v>
       </c>
       <c r="B55">
         <v>176</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>5.681818181818182E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>85</v>
       </c>
       <c r="B56">
         <v>156</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>6.41025641025641E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>85</v>
       </c>
       <c r="B57">
         <v>161</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>6.2111801242236021E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>85</v>
       </c>
       <c r="B58">
         <v>164</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>6.0975609756097563E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>90</v>
       </c>
       <c r="B59">
         <v>144</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>6.9444444444444441E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>90</v>
       </c>
       <c r="B60">
         <v>144</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C60">
+        <f t="shared" si="0"/>
+        <v>6.9444444444444441E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>90</v>
       </c>
       <c r="B61">
         <v>147</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>6.8027210884353739E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>95</v>
       </c>
       <c r="B62">
         <v>125</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C62">
+        <f t="shared" si="0"/>
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>95</v>
       </c>
       <c r="B63">
         <v>135</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C63">
+        <f t="shared" si="0"/>
+        <v>7.4074074074074077E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>95</v>
       </c>
       <c r="B64">
         <v>134</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C64">
+        <f t="shared" si="0"/>
+        <v>7.462686567164179E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>100</v>
       </c>
       <c r="B65">
         <v>135</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C65">
+        <f t="shared" si="0"/>
+        <v>7.4074074074074077E-3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>100</v>
       </c>
       <c r="B66">
         <v>136</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C66">
+        <f t="shared" si="0"/>
+        <v>7.3529411764705881E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>100</v>
       </c>
       <c r="B67">
         <v>131</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C67">
+        <f t="shared" ref="C67:C94" si="1">1/B67</f>
+        <v>7.6335877862595417E-3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>105</v>
       </c>
       <c r="B68">
         <v>123</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C68">
+        <f t="shared" si="1"/>
+        <v>8.130081300813009E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>105</v>
       </c>
       <c r="B69">
         <v>127</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C69">
+        <f t="shared" si="1"/>
+        <v>7.874015748031496E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>105</v>
       </c>
       <c r="B70">
         <v>128</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C70">
+        <f t="shared" si="1"/>
+        <v>7.8125E-3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>110</v>
       </c>
       <c r="B71">
         <v>123</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C71">
+        <f t="shared" si="1"/>
+        <v>8.130081300813009E-3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>110</v>
       </c>
       <c r="B72">
         <v>129</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C72">
+        <f t="shared" si="1"/>
+        <v>7.7519379844961239E-3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>110</v>
       </c>
       <c r="B73">
         <v>115</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C73">
+        <f t="shared" si="1"/>
+        <v>8.6956521739130436E-3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>115</v>
       </c>
       <c r="B74">
         <v>120</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C74">
+        <f t="shared" si="1"/>
+        <v>8.3333333333333332E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>115</v>
       </c>
       <c r="B75">
         <v>120</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C75">
+        <f t="shared" si="1"/>
+        <v>8.3333333333333332E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>115</v>
       </c>
       <c r="B76">
         <v>121</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C76">
+        <f t="shared" si="1"/>
+        <v>8.2644628099173556E-3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>120</v>
       </c>
       <c r="B77">
         <v>117</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C77">
+        <f t="shared" si="1"/>
+        <v>8.5470085470085479E-3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>120</v>
       </c>
       <c r="B78">
         <v>124</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C78">
+        <f t="shared" si="1"/>
+        <v>8.0645161290322578E-3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>120</v>
       </c>
       <c r="B79">
         <v>112</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C79">
+        <f t="shared" si="1"/>
+        <v>8.9285714285714281E-3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>125</v>
       </c>
       <c r="B80">
         <v>93</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C80">
+        <f t="shared" si="1"/>
+        <v>1.0752688172043012E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>125</v>
       </c>
       <c r="B81">
         <v>100</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C81">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>125</v>
       </c>
       <c r="B82">
         <v>110</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C82">
+        <f t="shared" si="1"/>
+        <v>9.0909090909090905E-3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>125</v>
       </c>
       <c r="B83">
         <v>112</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C83">
+        <f t="shared" si="1"/>
+        <v>8.9285714285714281E-3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>125</v>
       </c>
       <c r="B84">
         <v>117</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C84">
+        <f t="shared" si="1"/>
+        <v>8.5470085470085479E-3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>125</v>
       </c>
       <c r="B85">
         <v>110</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C85">
+        <f t="shared" si="1"/>
+        <v>9.0909090909090905E-3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>130</v>
       </c>
       <c r="B86">
         <v>104</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C86">
+        <f t="shared" si="1"/>
+        <v>9.6153846153846159E-3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>130</v>
       </c>
       <c r="B87">
         <v>103</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C87">
+        <f t="shared" si="1"/>
+        <v>9.7087378640776691E-3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>130</v>
       </c>
       <c r="B88">
         <v>107</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C88">
+        <f t="shared" si="1"/>
+        <v>9.3457943925233638E-3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>135</v>
       </c>
       <c r="B89">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+      <c r="C89">
+        <f>1/B89</f>
+        <v>9.5238095238095247E-3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>135</v>
       </c>
       <c r="B90">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+      <c r="C90">
+        <f t="shared" ref="C90:C94" si="2">1/B90</f>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>135</v>
       </c>
       <c r="B91">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+      <c r="C91">
+        <f t="shared" si="2"/>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>140</v>
       </c>
       <c r="B92">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+      <c r="C92">
+        <f t="shared" si="2"/>
+        <v>1.1764705882352941E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>140</v>
       </c>
       <c r="B93">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+      <c r="C93">
+        <f t="shared" si="2"/>
+        <v>1.1363636363636364E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>140</v>
       </c>
       <c r="B94">
-        <v>100</v>
+        <v>85</v>
+      </c>
+      <c r="C94">
+        <f t="shared" si="2"/>
+        <v>1.1764705882352941E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>